<commit_message>
update leave card 2/7/2024 8:56am
</commit_message>
<xml_diff>
--- a/CASUAL/LA PICNIC GROVE/CASTRENCE, DELIA M..xlsx
+++ b/CASUAL/LA PICNIC GROVE/CASTRENCE, DELIA M..xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="60">
   <si>
     <t>PERIOD</t>
   </si>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t>UT(0-1-30)</t>
+  </si>
+  <si>
+    <t>2024</t>
   </si>
 </sst>
 </file>
@@ -606,6 +609,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -618,20 +630,11 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1328,7 +1331,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1371,7 +1374,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1435,7 +1438,7 @@
         <xdr:cNvPr id="4" name="Arrow: Left 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1495,7 +1498,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1561,7 +1564,7 @@
         <xdr:cNvPr id="9" name="Arrow: Left-Right 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1624,7 +1627,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1722,7 +1725,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1781,7 +1784,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1846,7 +1849,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1889,7 +1892,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1964,7 +1967,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2150,7 +2153,7 @@
         <xdr:cNvPr id="23" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2216,7 +2219,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2274,7 +2277,7 @@
         <xdr:cNvPr id="26" name="Oval 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2340,7 +2343,7 @@
         <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2396,7 +2399,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2471,7 +2474,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2514,7 +2517,7 @@
         <xdr:cNvPr id="32" name="Oval 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2580,7 +2583,7 @@
         <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2636,7 +2639,7 @@
         <xdr:cNvPr id="34" name="TextBox 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2734,7 +2737,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C99D8E5F-2D60-FF91-2593-A29CC276458B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C99D8E5F-2D60-FF91-2593-A29CC276458B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2797,7 +2800,7 @@
         <xdr:cNvPr id="3" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D7E6A331-FC2C-4EF9-8F5B-65908D453D1C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7E6A331-FC2C-4EF9-8F5B-65908D453D1C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2863,7 +2866,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A8:K135" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A8:K136" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
   <tableColumns count="11">
     <tableColumn id="1" name="PERIOD" dataDxfId="35"/>
     <tableColumn id="2" name="PARTICULARS" dataDxfId="34"/>
@@ -3271,12 +3274,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:K135"/>
+  <dimension ref="A2:K136"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4785" topLeftCell="A61" activePane="bottomLeft"/>
+      <pane ySplit="4785" topLeftCell="A82" activePane="bottomLeft"/>
       <selection activeCell="F4" sqref="F4:G4"/>
-      <selection pane="bottomLeft" activeCell="E71" sqref="E71"/>
+      <selection pane="bottomLeft" activeCell="E90" sqref="E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3306,14 +3309,14 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="55"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -3324,16 +3327,16 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="53">
+      <c r="F3" s="56">
         <v>42020</v>
       </c>
-      <c r="G3" s="54"/>
+      <c r="G3" s="50"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="58"/>
     </row>
     <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
@@ -3346,14 +3349,14 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="57"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="51"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
@@ -3379,18 +3382,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58" t="s">
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3437,7 +3440,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table15[EARNED])-SUM(Table15[Absence Undertime W/ Pay])</f>
-        <v>61.003</v>
+        <v>64.753</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -3447,7 +3450,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table15[[EARNED ]])-SUM(Table15[Absence Undertime  W/ Pay])</f>
-        <v>87.5</v>
+        <v>91.25</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
@@ -5037,13 +5040,15 @@
         <v>45231</v>
       </c>
       <c r="B87" s="20"/>
-      <c r="C87" s="13"/>
+      <c r="C87" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D87" s="39"/>
       <c r="E87" s="9"/>
       <c r="F87" s="20"/>
-      <c r="G87" s="13" t="str">
-        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G87" s="13">
+        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H87" s="39"/>
       <c r="I87" s="9"/>
@@ -5055,13 +5060,15 @@
         <v>45261</v>
       </c>
       <c r="B88" s="20"/>
-      <c r="C88" s="13"/>
+      <c r="C88" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D88" s="39"/>
       <c r="E88" s="9"/>
       <c r="F88" s="20"/>
-      <c r="G88" s="13" t="str">
-        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G88" s="13">
+        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H88" s="39"/>
       <c r="I88" s="9"/>
@@ -5069,33 +5076,34 @@
       <c r="K88" s="20"/>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A89" s="40">
-        <v>45292</v>
+      <c r="A89" s="48" t="s">
+        <v>59</v>
       </c>
       <c r="B89" s="20"/>
       <c r="C89" s="13"/>
       <c r="D89" s="39"/>
       <c r="E89" s="9"/>
       <c r="F89" s="20"/>
-      <c r="G89" s="13" t="str">
-        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
+      <c r="G89" s="13"/>
       <c r="H89" s="39"/>
       <c r="I89" s="9"/>
       <c r="J89" s="11"/>
       <c r="K89" s="20"/>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A90" s="40"/>
+      <c r="A90" s="40">
+        <v>45292</v>
+      </c>
       <c r="B90" s="20"/>
-      <c r="C90" s="13"/>
+      <c r="C90" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D90" s="39"/>
       <c r="E90" s="9"/>
       <c r="F90" s="20"/>
-      <c r="G90" s="13" t="str">
-        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G90" s="13">
+        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H90" s="39"/>
       <c r="I90" s="9"/>
@@ -5807,34 +5815,50 @@
       <c r="K134" s="20"/>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A135" s="41"/>
-      <c r="B135" s="15"/>
-      <c r="C135" s="42"/>
-      <c r="D135" s="43"/>
+      <c r="A135" s="40"/>
+      <c r="B135" s="20"/>
+      <c r="C135" s="13"/>
+      <c r="D135" s="39"/>
       <c r="E135" s="9"/>
-      <c r="F135" s="15"/>
-      <c r="G135" s="42" t="str">
-        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H135" s="43"/>
+      <c r="F135" s="20"/>
+      <c r="G135" s="13" t="str">
+        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H135" s="39"/>
       <c r="I135" s="9"/>
-      <c r="J135" s="12"/>
-      <c r="K135" s="15"/>
+      <c r="J135" s="11"/>
+      <c r="K135" s="20"/>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A136" s="41"/>
+      <c r="B136" s="15"/>
+      <c r="C136" s="42"/>
+      <c r="D136" s="43"/>
+      <c r="E136" s="9"/>
+      <c r="F136" s="15"/>
+      <c r="G136" s="42" t="str">
+        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H136" s="43"/>
+      <c r="I136" s="9"/>
+      <c r="J136" s="12"/>
+      <c r="K136" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
@@ -5903,14 +5927,14 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="55"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -5924,17 +5948,17 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="53">
+      <c r="F3" s="56">
         <f>IF(ISBLANK('2018 LEAVE CREDITS'!F3:G3),"---------",'2018 LEAVE CREDITS'!F3:G3)</f>
         <v>42020</v>
       </c>
-      <c r="G3" s="54"/>
+      <c r="G3" s="50"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="58"/>
     </row>
     <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
@@ -5948,17 +5972,17 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="54" t="str">
+      <c r="F4" s="50" t="str">
         <f>IF(ISBLANK('2018 LEAVE CREDITS'!F4:G4),"",'2018 LEAVE CREDITS'!F4:G4)</f>
         <v/>
       </c>
-      <c r="G4" s="54"/>
+      <c r="G4" s="50"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="57"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="51"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
@@ -5984,18 +6008,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58" t="s">
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -8169,7 +8193,7 @@
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <f>SUM('2018 LEAVE CREDITS'!E9,'2018 LEAVE CREDITS'!I9)</f>
-        <v>148.50299999999999</v>
+        <v>156.00299999999999</v>
       </c>
       <c r="C7" s="37">
         <v>1</v>

</xml_diff>